<commit_message>
Add QS code to quantity survey import
</commit_message>
<xml_diff>
--- a/public/files/templates/qs.xlsx
+++ b/public/files/templates/qs.xlsx
@@ -16,7 +16,7 @@
     <sheet name="SUM QS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$G$2</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>WBS-Code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Description</t>
   </si>
@@ -48,7 +45,13 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Item Code</t>
+    <t>BOQ item code</t>
+  </si>
+  <si>
+    <t>QS Item Code</t>
+  </si>
+  <si>
+    <t>WBS Code</t>
   </si>
 </sst>
 </file>
@@ -102,11 +105,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:F2"/>
-  <tableColumns count="6">
-    <tableColumn id="2" name="WBS-Code"/>
-    <tableColumn id="1" name="Item Code"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:G2"/>
+  <tableColumns count="7">
+    <tableColumn id="2" name="WBS Code"/>
+    <tableColumn id="1" name="BOQ item code"/>
+    <tableColumn id="7" name="QS Item Code"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="4" name="Budget Quantity"/>
     <tableColumn id="5" name="Engineer Quantity"/>
@@ -403,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -412,31 +416,35 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="57.1640625" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>